<commit_message>
CRUD Driver, Truck, Trailer, Load
</commit_message>
<xml_diff>
--- a/staticfiles/2025_SafetyDepartment.xlsx
+++ b/staticfiles/2025_SafetyDepartment.xlsx
@@ -1783,8 +1783,8 @@
   </sheetPr>
   <dimension ref="A1:U1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1796,10 +1796,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="4.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16375" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16375" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1829,16 +1829,16 @@
       </c>
       <c r="J1" s="4"/>
       <c r="K1" s="1"/>
-      <c r="L1" s="0"/>
-      <c r="M1" s="0"/>
-      <c r="N1" s="0"/>
-      <c r="O1" s="0"/>
-      <c r="P1" s="0"/>
-      <c r="Q1" s="0"/>
-      <c r="R1" s="0"/>
-      <c r="S1" s="0"/>
-      <c r="T1" s="0"/>
-      <c r="U1" s="0"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
     </row>
     <row r="2" s="5" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="6"/>
@@ -1868,16 +1868,16 @@
       </c>
       <c r="J2" s="9"/>
       <c r="K2" s="1"/>
-      <c r="L2" s="0"/>
-      <c r="M2" s="0"/>
-      <c r="N2" s="0"/>
-      <c r="O2" s="0"/>
-      <c r="P2" s="0"/>
-      <c r="Q2" s="0"/>
-      <c r="R2" s="0"/>
-      <c r="S2" s="0"/>
-      <c r="T2" s="0"/>
-      <c r="U2" s="0"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6"/>
@@ -1907,16 +1907,16 @@
       </c>
       <c r="J3" s="9"/>
       <c r="K3" s="1"/>
-      <c r="L3" s="0"/>
-      <c r="M3" s="0"/>
-      <c r="N3" s="0"/>
-      <c r="O3" s="0"/>
-      <c r="P3" s="0"/>
-      <c r="Q3" s="0"/>
-      <c r="R3" s="0"/>
-      <c r="S3" s="0"/>
-      <c r="T3" s="0"/>
-      <c r="U3" s="0"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
     </row>
     <row r="4" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
@@ -1946,16 +1946,16 @@
       </c>
       <c r="J4" s="9"/>
       <c r="K4" s="1"/>
-      <c r="L4" s="0"/>
-      <c r="M4" s="0"/>
-      <c r="N4" s="0"/>
-      <c r="O4" s="0"/>
-      <c r="P4" s="0"/>
-      <c r="Q4" s="0"/>
-      <c r="R4" s="0"/>
-      <c r="S4" s="0"/>
-      <c r="T4" s="0"/>
-      <c r="U4" s="0"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
     </row>
     <row r="5" s="5" customFormat="true" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
@@ -1985,16 +1985,16 @@
       </c>
       <c r="J5" s="9"/>
       <c r="K5" s="1"/>
-      <c r="L5" s="0"/>
-      <c r="M5" s="0"/>
-      <c r="N5" s="0"/>
-      <c r="O5" s="0"/>
-      <c r="P5" s="0"/>
-      <c r="Q5" s="0"/>
-      <c r="R5" s="0"/>
-      <c r="S5" s="0"/>
-      <c r="T5" s="0"/>
-      <c r="U5" s="0"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
     </row>
     <row r="6" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
@@ -2024,16 +2024,16 @@
       </c>
       <c r="J6" s="9"/>
       <c r="K6" s="1"/>
-      <c r="L6" s="0"/>
-      <c r="M6" s="0"/>
-      <c r="N6" s="0"/>
-      <c r="O6" s="0"/>
-      <c r="P6" s="0"/>
-      <c r="Q6" s="0"/>
-      <c r="R6" s="0"/>
-      <c r="S6" s="0"/>
-      <c r="T6" s="0"/>
-      <c r="U6" s="0"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
     </row>
     <row r="7" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
@@ -2063,16 +2063,16 @@
       </c>
       <c r="J7" s="9"/>
       <c r="K7" s="1"/>
-      <c r="L7" s="0"/>
-      <c r="M7" s="0"/>
-      <c r="N7" s="0"/>
-      <c r="O7" s="0"/>
-      <c r="P7" s="0"/>
-      <c r="Q7" s="0"/>
-      <c r="R7" s="0"/>
-      <c r="S7" s="0"/>
-      <c r="T7" s="0"/>
-      <c r="U7" s="0"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
     </row>
     <row r="8" s="5" customFormat="true" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
@@ -2102,16 +2102,16 @@
       </c>
       <c r="J8" s="9"/>
       <c r="K8" s="1"/>
-      <c r="L8" s="0"/>
-      <c r="M8" s="0"/>
-      <c r="N8" s="0"/>
-      <c r="O8" s="0"/>
-      <c r="P8" s="0"/>
-      <c r="Q8" s="0"/>
-      <c r="R8" s="0"/>
-      <c r="S8" s="0"/>
-      <c r="T8" s="0"/>
-      <c r="U8" s="0"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
     </row>
     <row r="9" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
@@ -2141,16 +2141,16 @@
       </c>
       <c r="J9" s="11"/>
       <c r="K9" s="1"/>
-      <c r="L9" s="0"/>
-      <c r="M9" s="0"/>
-      <c r="N9" s="0"/>
-      <c r="O9" s="0"/>
-      <c r="P9" s="0"/>
-      <c r="Q9" s="0"/>
-      <c r="R9" s="0"/>
-      <c r="S9" s="0"/>
-      <c r="T9" s="0"/>
-      <c r="U9" s="0"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
@@ -2180,16 +2180,16 @@
       </c>
       <c r="J10" s="11"/>
       <c r="K10" s="1"/>
-      <c r="L10" s="0"/>
-      <c r="M10" s="0"/>
-      <c r="N10" s="0"/>
-      <c r="O10" s="0"/>
-      <c r="P10" s="0"/>
-      <c r="Q10" s="0"/>
-      <c r="R10" s="0"/>
-      <c r="S10" s="0"/>
-      <c r="T10" s="0"/>
-      <c r="U10" s="0"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
     </row>
     <row r="11" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="12"/>
@@ -2219,16 +2219,16 @@
       </c>
       <c r="J11" s="11"/>
       <c r="K11" s="1"/>
-      <c r="L11" s="0"/>
-      <c r="M11" s="0"/>
-      <c r="N11" s="0"/>
-      <c r="O11" s="0"/>
-      <c r="P11" s="0"/>
-      <c r="Q11" s="0"/>
-      <c r="R11" s="0"/>
-      <c r="S11" s="0"/>
-      <c r="T11" s="0"/>
-      <c r="U11" s="0"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
     </row>
     <row r="12" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6"/>
@@ -2258,16 +2258,16 @@
       </c>
       <c r="J12" s="9"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="0"/>
-      <c r="M12" s="0"/>
-      <c r="N12" s="0"/>
-      <c r="O12" s="0"/>
-      <c r="P12" s="0"/>
-      <c r="Q12" s="0"/>
-      <c r="R12" s="0"/>
-      <c r="S12" s="0"/>
-      <c r="T12" s="0"/>
-      <c r="U12" s="0"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
     </row>
     <row r="13" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="13"/>
@@ -2297,16 +2297,16 @@
       </c>
       <c r="J13" s="11"/>
       <c r="K13" s="1"/>
-      <c r="L13" s="0"/>
-      <c r="M13" s="0"/>
-      <c r="N13" s="0"/>
-      <c r="O13" s="0"/>
-      <c r="P13" s="0"/>
-      <c r="Q13" s="0"/>
-      <c r="R13" s="0"/>
-      <c r="S13" s="0"/>
-      <c r="T13" s="0"/>
-      <c r="U13" s="0"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
     </row>
     <row r="14" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="12"/>
@@ -2336,16 +2336,16 @@
       </c>
       <c r="J14" s="11"/>
       <c r="K14" s="1"/>
-      <c r="L14" s="0"/>
-      <c r="M14" s="0"/>
-      <c r="N14" s="0"/>
-      <c r="O14" s="0"/>
-      <c r="P14" s="0"/>
-      <c r="Q14" s="0"/>
-      <c r="R14" s="0"/>
-      <c r="S14" s="0"/>
-      <c r="T14" s="0"/>
-      <c r="U14" s="0"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
     </row>
     <row r="15" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6"/>
@@ -2375,16 +2375,16 @@
       </c>
       <c r="J15" s="11"/>
       <c r="K15" s="1"/>
-      <c r="L15" s="0"/>
-      <c r="M15" s="0"/>
-      <c r="N15" s="0"/>
-      <c r="O15" s="0"/>
-      <c r="P15" s="0"/>
-      <c r="Q15" s="0"/>
-      <c r="R15" s="0"/>
-      <c r="S15" s="0"/>
-      <c r="T15" s="0"/>
-      <c r="U15" s="0"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
     </row>
     <row r="16" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6"/>
@@ -2414,16 +2414,16 @@
       </c>
       <c r="J16" s="11"/>
       <c r="K16" s="1"/>
-      <c r="L16" s="0"/>
-      <c r="M16" s="0"/>
-      <c r="N16" s="0"/>
-      <c r="O16" s="0"/>
-      <c r="P16" s="0"/>
-      <c r="Q16" s="0"/>
-      <c r="R16" s="0"/>
-      <c r="S16" s="0"/>
-      <c r="T16" s="0"/>
-      <c r="U16" s="0"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
     </row>
     <row r="17" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6"/>
@@ -2453,16 +2453,16 @@
       </c>
       <c r="J17" s="9"/>
       <c r="K17" s="1"/>
-      <c r="L17" s="0"/>
-      <c r="M17" s="0"/>
-      <c r="N17" s="0"/>
-      <c r="O17" s="0"/>
-      <c r="P17" s="0"/>
-      <c r="Q17" s="0"/>
-      <c r="R17" s="0"/>
-      <c r="S17" s="0"/>
-      <c r="T17" s="0"/>
-      <c r="U17" s="0"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
     </row>
     <row r="18" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="12"/>
@@ -2492,16 +2492,16 @@
       </c>
       <c r="J18" s="11"/>
       <c r="K18" s="1"/>
-      <c r="L18" s="0"/>
-      <c r="M18" s="0"/>
-      <c r="N18" s="0"/>
-      <c r="O18" s="0"/>
-      <c r="P18" s="0"/>
-      <c r="Q18" s="0"/>
-      <c r="R18" s="0"/>
-      <c r="S18" s="0"/>
-      <c r="T18" s="0"/>
-      <c r="U18" s="0"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
     </row>
     <row r="19" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6"/>
@@ -2531,16 +2531,16 @@
       </c>
       <c r="J19" s="9"/>
       <c r="K19" s="1"/>
-      <c r="L19" s="0"/>
-      <c r="M19" s="0"/>
-      <c r="N19" s="0"/>
-      <c r="O19" s="0"/>
-      <c r="P19" s="0"/>
-      <c r="Q19" s="0"/>
-      <c r="R19" s="0"/>
-      <c r="S19" s="0"/>
-      <c r="T19" s="0"/>
-      <c r="U19" s="0"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
     </row>
     <row r="20" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6"/>
@@ -2570,16 +2570,16 @@
       </c>
       <c r="J20" s="11"/>
       <c r="K20" s="1"/>
-      <c r="L20" s="0"/>
-      <c r="M20" s="0"/>
-      <c r="N20" s="0"/>
-      <c r="O20" s="0"/>
-      <c r="P20" s="0"/>
-      <c r="Q20" s="0"/>
-      <c r="R20" s="0"/>
-      <c r="S20" s="0"/>
-      <c r="T20" s="0"/>
-      <c r="U20" s="0"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="17"/>
@@ -11094,8 +11094,8 @@
   </sheetPr>
   <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11110,7 +11110,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="20" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="20" width="12.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="10" style="20" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="92.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -22592,7 +22592,7 @@
   <dimension ref="A1:T1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22605,7 +22605,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="22" width="7.29"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="22" width="12.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="19" min="9" style="23" width="12.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -22642,7 +22642,7 @@
       <c r="Q1" s="26"/>
       <c r="R1" s="26"/>
       <c r="S1" s="26"/>
-      <c r="T1" s="0"/>
+      <c r="T1" s="1"/>
     </row>
     <row r="2" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
@@ -22678,7 +22678,7 @@
       <c r="Q2" s="26"/>
       <c r="R2" s="26"/>
       <c r="S2" s="26"/>
-      <c r="T2" s="0"/>
+      <c r="T2" s="1"/>
     </row>
     <row r="3" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
@@ -22714,7 +22714,7 @@
       <c r="Q3" s="26"/>
       <c r="R3" s="26"/>
       <c r="S3" s="26"/>
-      <c r="T3" s="0"/>
+      <c r="T3" s="1"/>
     </row>
     <row r="4" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="7" t="n">
@@ -22750,7 +22750,7 @@
       <c r="Q4" s="26"/>
       <c r="R4" s="26"/>
       <c r="S4" s="26"/>
-      <c r="T4" s="0"/>
+      <c r="T4" s="1"/>
     </row>
     <row r="5" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7" t="n">
@@ -22786,7 +22786,7 @@
       <c r="Q5" s="26"/>
       <c r="R5" s="26"/>
       <c r="S5" s="26"/>
-      <c r="T5" s="0"/>
+      <c r="T5" s="1"/>
     </row>
     <row r="6" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
@@ -22822,7 +22822,7 @@
       <c r="Q6" s="26"/>
       <c r="R6" s="26"/>
       <c r="S6" s="26"/>
-      <c r="T6" s="0"/>
+      <c r="T6" s="1"/>
     </row>
     <row r="7" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="n">
@@ -22858,7 +22858,7 @@
       <c r="Q7" s="26"/>
       <c r="R7" s="26"/>
       <c r="S7" s="26"/>
-      <c r="T7" s="0"/>
+      <c r="T7" s="1"/>
     </row>
     <row r="8" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
@@ -22894,7 +22894,7 @@
       <c r="Q8" s="26"/>
       <c r="R8" s="26"/>
       <c r="S8" s="26"/>
-      <c r="T8" s="0"/>
+      <c r="T8" s="1"/>
     </row>
     <row r="9" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="n">
@@ -22930,7 +22930,7 @@
       <c r="Q9" s="26"/>
       <c r="R9" s="26"/>
       <c r="S9" s="26"/>
-      <c r="T9" s="0"/>
+      <c r="T9" s="1"/>
     </row>
     <row r="10" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
@@ -22966,7 +22966,7 @@
       <c r="Q10" s="26"/>
       <c r="R10" s="26"/>
       <c r="S10" s="26"/>
-      <c r="T10" s="0"/>
+      <c r="T10" s="1"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">

</xml_diff>